<commit_message>
Tracking work on resources labs
</commit_message>
<xml_diff>
--- a/resources/labs/test_cases.xlsx
+++ b/resources/labs/test_cases.xlsx
@@ -275,8 +275,36 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -328,7 +356,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -433,7 +460,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -633,7 +659,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -776,11 +801,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="445036080"/>
-        <c:axId val="445008880"/>
+        <c:axId val="2062975056"/>
+        <c:axId val="2062979408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445036080"/>
+        <c:axId val="2062975056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="445008880"/>
+        <c:crossAx val="2062979408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -831,7 +856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445008880"/>
+        <c:axId val="2062979408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +892,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445036080"/>
+        <c:crossAx val="2062975056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -881,7 +906,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1879,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>